<commit_message>
rename particle to component and tweak Dockerfile for plotly
</commit_message>
<xml_diff>
--- a/input/concentrations/ds.5p/data.input.xlsx
+++ b/input/concentrations/ds.5p/data.input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\ds.5p\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\concentrations\ds.5p\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF34BA0-146B-4B49-983C-C6B5B677FED1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFB4FD8-DC47-454D-9C33-612D3D6E3268}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="stoich_coefficients" sheetId="1" r:id="rId1"/>
     <sheet name="concentrations" sheetId="2" r:id="rId2"/>
     <sheet name="k_constants_log10" sheetId="3" r:id="rId3"/>
-    <sheet name="particle_names" sheetId="6" r:id="rId4"/>
+    <sheet name="component_names" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>